<commit_message>
anim file + simulation result file add
</commit_message>
<xml_diff>
--- a/data/データ分析(損失原因)_4_26.xlsx
+++ b/data/データ分析(損失原因)_4_26.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shuto\ns3.30\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DBE60CF-E40F-449F-B177-780DCEEA2093}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DE0AF1EC-2071-4D96-BBE0-1A270B7B0457}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1757" yWindow="2014" windowWidth="12343" windowHeight="6395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="6">
   <si>
     <t>Seed</t>
     <phoneticPr fontId="1"/>
@@ -66,10 +67,6 @@
     <rPh sb="9" eb="10">
       <t>カズ</t>
     </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>SUM</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -414,8 +411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:O38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.45"/>
@@ -439,7 +436,7 @@
         <v>500</v>
       </c>
       <c r="O1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="2:15">
@@ -477,13 +474,22 @@
         <v>0</v>
       </c>
       <c r="O2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="2:15">
       <c r="B3">
         <v>10000</v>
       </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
       <c r="F3">
         <v>2</v>
       </c>
@@ -510,6 +516,15 @@
       <c r="B4">
         <v>20000</v>
       </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
       <c r="F4">
         <v>1</v>
       </c>
@@ -536,6 +551,24 @@
       <c r="B5">
         <v>30000</v>
       </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
       <c r="I5">
         <v>2</v>
       </c>
@@ -553,6 +586,24 @@
       <c r="B6">
         <v>40000</v>
       </c>
+      <c r="C6">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
       <c r="I6">
         <v>1</v>
       </c>
@@ -570,6 +621,15 @@
       <c r="B7">
         <v>50000</v>
       </c>
+      <c r="F7">
+        <v>3</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
       <c r="I7">
         <v>1</v>
       </c>
@@ -587,6 +647,15 @@
       <c r="B8">
         <v>60000</v>
       </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
       <c r="I8">
         <v>0</v>
       </c>
@@ -604,6 +673,15 @@
       <c r="B9">
         <v>70000</v>
       </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9">
+        <v>2</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
       <c r="I9">
         <v>1</v>
       </c>
@@ -621,6 +699,15 @@
       <c r="B10">
         <v>80000</v>
       </c>
+      <c r="F10">
+        <v>3</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
       <c r="I10">
         <v>2</v>
       </c>
@@ -638,6 +725,15 @@
       <c r="B11">
         <v>90000</v>
       </c>
+      <c r="F11">
+        <v>3</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
       <c r="I11">
         <v>1</v>
       </c>
@@ -655,6 +751,15 @@
       <c r="B12">
         <v>11000</v>
       </c>
+      <c r="F12">
+        <v>3</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
       <c r="I12">
         <v>1</v>
       </c>
@@ -672,6 +777,15 @@
       <c r="B13">
         <v>22000</v>
       </c>
+      <c r="F13">
+        <v>3</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
       <c r="I13">
         <v>1</v>
       </c>
@@ -689,6 +803,15 @@
       <c r="B14">
         <v>33000</v>
       </c>
+      <c r="F14">
+        <v>5</v>
+      </c>
+      <c r="G14">
+        <v>2</v>
+      </c>
+      <c r="H14">
+        <v>2</v>
+      </c>
       <c r="I14">
         <v>2</v>
       </c>
@@ -706,6 +829,15 @@
       <c r="B15">
         <v>44000</v>
       </c>
+      <c r="F15">
+        <v>2</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
       <c r="I15">
         <v>4</v>
       </c>
@@ -723,6 +855,15 @@
       <c r="B16">
         <v>55000</v>
       </c>
+      <c r="F16">
+        <v>2</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
       <c r="I16">
         <v>1</v>
       </c>
@@ -740,6 +881,15 @@
       <c r="B17">
         <v>66000</v>
       </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
       <c r="I17">
         <v>1</v>
       </c>
@@ -757,6 +907,15 @@
       <c r="B18">
         <v>77000</v>
       </c>
+      <c r="F18">
+        <v>2</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
       <c r="I18">
         <v>1</v>
       </c>
@@ -774,6 +933,15 @@
       <c r="B19">
         <v>88000</v>
       </c>
+      <c r="F19">
+        <v>3</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
       <c r="I19">
         <v>1</v>
       </c>
@@ -791,6 +959,15 @@
       <c r="B20">
         <v>99000</v>
       </c>
+      <c r="F20">
+        <v>3</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
       <c r="I20">
         <v>3</v>
       </c>
@@ -808,6 +985,15 @@
       <c r="B21">
         <v>11100</v>
       </c>
+      <c r="F21">
+        <v>2</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
       <c r="I21">
         <v>1</v>
       </c>
@@ -825,6 +1011,15 @@
       <c r="B22">
         <v>22200</v>
       </c>
+      <c r="F22">
+        <v>2</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
       <c r="I22">
         <v>2</v>
       </c>
@@ -842,6 +1037,15 @@
       <c r="B23">
         <v>33300</v>
       </c>
+      <c r="F23">
+        <v>4</v>
+      </c>
+      <c r="G23">
+        <v>2</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
       <c r="I23">
         <v>1</v>
       </c>
@@ -859,6 +1063,15 @@
       <c r="B24">
         <v>44400</v>
       </c>
+      <c r="F24">
+        <v>2</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
       <c r="I24">
         <v>2</v>
       </c>
@@ -876,6 +1089,15 @@
       <c r="B25">
         <v>55500</v>
       </c>
+      <c r="F25">
+        <v>2</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
       <c r="I25">
         <v>2</v>
       </c>
@@ -893,6 +1115,15 @@
       <c r="B26">
         <v>66600</v>
       </c>
+      <c r="F26">
+        <v>3</v>
+      </c>
+      <c r="G26">
+        <v>2</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
       <c r="I26">
         <v>2</v>
       </c>
@@ -910,6 +1141,15 @@
       <c r="B27">
         <v>77700</v>
       </c>
+      <c r="F27">
+        <v>2</v>
+      </c>
+      <c r="G27">
+        <v>2</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
       <c r="I27">
         <v>1</v>
       </c>
@@ -927,6 +1167,15 @@
       <c r="B28">
         <v>88800</v>
       </c>
+      <c r="F28">
+        <v>4</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
       <c r="I28">
         <v>1</v>
       </c>
@@ -944,6 +1193,15 @@
       <c r="B29">
         <v>99900</v>
       </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
       <c r="I29">
         <v>3</v>
       </c>
@@ -961,6 +1219,15 @@
       <c r="B30">
         <v>11110</v>
       </c>
+      <c r="F30">
+        <v>5</v>
+      </c>
+      <c r="G30">
+        <v>2</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
       <c r="I30">
         <v>1</v>
       </c>
@@ -978,6 +1245,15 @@
       <c r="B31">
         <v>22220</v>
       </c>
+      <c r="F31">
+        <v>3</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
       <c r="I31">
         <v>1</v>
       </c>
@@ -995,6 +1271,15 @@
       <c r="B32">
         <v>33330</v>
       </c>
+      <c r="F32">
+        <v>2</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
       <c r="I32">
         <v>1</v>
       </c>
@@ -1012,6 +1297,15 @@
       <c r="B33">
         <v>44440</v>
       </c>
+      <c r="F33">
+        <v>3</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
       <c r="I33">
         <v>1</v>
       </c>
@@ -1029,6 +1323,15 @@
       <c r="B34">
         <v>55550</v>
       </c>
+      <c r="F34">
+        <v>5</v>
+      </c>
+      <c r="G34">
+        <v>2</v>
+      </c>
+      <c r="H34">
+        <v>1</v>
+      </c>
       <c r="I34">
         <v>0</v>
       </c>
@@ -1046,6 +1349,15 @@
       <c r="B35">
         <v>66660</v>
       </c>
+      <c r="F35">
+        <v>1</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
       <c r="I35">
         <v>0</v>
       </c>
@@ -1063,6 +1375,15 @@
       <c r="B36">
         <v>77770</v>
       </c>
+      <c r="F36">
+        <v>4</v>
+      </c>
+      <c r="G36">
+        <v>3</v>
+      </c>
+      <c r="H36">
+        <v>3</v>
+      </c>
       <c r="I36">
         <v>4</v>
       </c>
@@ -1080,6 +1401,15 @@
       <c r="B37">
         <v>88880</v>
       </c>
+      <c r="F37">
+        <v>4</v>
+      </c>
+      <c r="G37">
+        <v>3</v>
+      </c>
+      <c r="H37">
+        <v>2</v>
+      </c>
       <c r="I37">
         <v>2</v>
       </c>
@@ -1094,15 +1424,24 @@
       </c>
     </row>
     <row r="38" spans="2:12">
-      <c r="B38" t="s">
-        <v>4</v>
+      <c r="F38">
+        <f t="shared" ref="F38:K38" si="0">SUM(F3:F37)</f>
+        <v>91</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="0"/>
+        <v>24</v>
       </c>
       <c r="I38">
-        <f>SUM(I3:I37)</f>
+        <f t="shared" si="0"/>
         <v>51</v>
       </c>
       <c r="J38">
-        <f t="shared" ref="J38:K38" si="0">SUM(J3:J37)</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="K38">

</xml_diff>